<commit_message>
added required keywords to alumnus.xlsx
</commit_message>
<xml_diff>
--- a/apps/website/static/files/alumnus.xlsx
+++ b/apps/website/static/files/alumnus.xlsx
@@ -24,15 +24,6 @@
     <t>Gender</t>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>First name</t>
-  </si>
-  <si>
-    <t>Last name</t>
-  </si>
-  <si>
     <t>Grad. Year</t>
   </si>
   <si>
@@ -46,6 +37,15 @@
   </si>
   <si>
     <t>Current State</t>
+  </si>
+  <si>
+    <t>Email (*Required)</t>
+  </si>
+  <si>
+    <t>First name (*Required)</t>
+  </si>
+  <si>
+    <t>Last name (*Required)</t>
   </si>
 </sst>
 </file>
@@ -455,12 +455,16 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
+    <col min="2" max="2" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="21.83203125" customWidth="1"/>
     <col min="7" max="7" width="19" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
@@ -469,31 +473,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:9">

</xml_diff>

<commit_message>
feature req: 'ability to export group to excel.' bug fix: 'add 3 step desc. for importing members through excel.'
</commit_message>
<xml_diff>
--- a/apps/website/static/files/alumnus.xlsx
+++ b/apps/website/static/files/alumnus.xlsx
@@ -80,9 +80,7 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -455,14 +453,14 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection sqref="A1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.5" customWidth="1"/>
-    <col min="2" max="2" width="20.6640625" customWidth="1"/>
-    <col min="3" max="3" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="3" max="3" width="24.5" customWidth="1"/>
     <col min="4" max="4" width="20.33203125" customWidth="1"/>
     <col min="5" max="5" width="22" customWidth="1"/>
     <col min="6" max="6" width="21.83203125" customWidth="1"/>

</xml_diff>

<commit_message>
bug fix: 'Participant type not present in excel import step'
</commit_message>
<xml_diff>
--- a/apps/website/static/files/alumnus.xlsx
+++ b/apps/website/static/files/alumnus.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="960" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Gender</t>
   </si>
@@ -46,6 +46,9 @@
   </si>
   <si>
     <t>Last name (*Required)</t>
+  </si>
+  <si>
+    <t>Participant Type</t>
   </si>
 </sst>
 </file>
@@ -100,7 +103,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -108,16 +111,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
@@ -450,10 +455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:I1"/>
+    <sheetView tabSelected="1" topLeftCell="A1047676" workbookViewId="0">
+      <selection activeCell="E1047684" sqref="E1047684"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -469,7 +474,7 @@
     <col min="9" max="9" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
@@ -480,31 +485,42 @@
         <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:10">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10">
       <c r="A3" s="1"/>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576">
+      <formula1>"Current Member, Past Member, Friend/Family of Member"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E1048576">
+      <formula1>"Male, Female"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>